<commit_message>
Update to nostradamus_v1.py trying to implement studytime metrics
</commit_message>
<xml_diff>
--- a/data for python CAT.xlsx
+++ b/data for python CAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/home/PycharmProjects/new code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE99653-D58E-1B42-BF0D-4683D8C997AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5691EEBF-6211-A644-9442-6FA6C58B11A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16800" activeTab="2" xr2:uid="{F108337B-EC49-3F49-91E9-C61B3B20BE64}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16800" xr2:uid="{F108337B-EC49-3F49-91E9-C61B3B20BE64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -543,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD242849-70F8-A241-90D3-7EB416C25FD5}">
   <dimension ref="A1:U417"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="101" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:O395"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -635,7 +635,6 @@
         <v>10</v>
       </c>
       <c r="M4">
-        <f>MAX(O1:O395)</f>
         <v>4</v>
       </c>
       <c r="O4" s="1">
@@ -12250,7 +12249,7 @@
         <v>0.75</v>
       </c>
       <c r="Q399">
-        <f t="shared" ref="Q399:Q462" si="25">(O385-M$3)/(M$4-M$3)</f>
+        <f t="shared" ref="Q399:Q409" si="25">(O385-M$3)/(M$4-M$3)</f>
         <v>0</v>
       </c>
     </row>
@@ -12548,6 +12547,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -12555,8 +12555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1A8AC44-04D8-A749-8DFB-B6500EBAADA5}">
   <dimension ref="A1:D396"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B396"/>
+    <sheetView topLeftCell="A363" workbookViewId="0">
+      <selection activeCell="B398" sqref="B398"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -19297,30 +19297,1997 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659F11ED-2DD7-FB4A-A0BD-C65056D1F598}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:J395"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:10">
       <c r="A1" s="4"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="J1" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="J2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="J3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="C4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="85">
+      <c r="J4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="J5" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="J6" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="J7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="J8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="J9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="J10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="J11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="85">
       <c r="F12" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="J12" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="F13" t="s">
         <v>17</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="J14" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="J15" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="10:10">
+      <c r="J17" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="10:10">
+      <c r="J18" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="10:10">
+      <c r="J19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="10:10">
+      <c r="J20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="10:10">
+      <c r="J21" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="10:10">
+      <c r="J22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="10:10">
+      <c r="J23" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="10:10">
+      <c r="J24" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="10:10">
+      <c r="J25" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="10:10">
+      <c r="J26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="10:10">
+      <c r="J27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="10:10">
+      <c r="J28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="10:10">
+      <c r="J29" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="10:10">
+      <c r="J30" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="10:10">
+      <c r="J31" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="10:10">
+      <c r="J32" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="10:10">
+      <c r="J33" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="10:10">
+      <c r="J34" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="10:10">
+      <c r="J35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="10:10">
+      <c r="J36" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="10:10">
+      <c r="J37" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="10:10">
+      <c r="J38" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="10:10">
+      <c r="J39" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="10:10">
+      <c r="J40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="10:10">
+      <c r="J41" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="10:10">
+      <c r="J42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="10:10">
+      <c r="J43" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="10:10">
+      <c r="J44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="10:10">
+      <c r="J45" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="10:10">
+      <c r="J46" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="10:10">
+      <c r="J47" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="10:10">
+      <c r="J48" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="10:10">
+      <c r="J49" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="10:10">
+      <c r="J50" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="10:10">
+      <c r="J51" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="10:10">
+      <c r="J52" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="10:10">
+      <c r="J53" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="10:10">
+      <c r="J54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="10:10">
+      <c r="J55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="10:10">
+      <c r="J56" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="10:10">
+      <c r="J57" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="10:10">
+      <c r="J58" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="10:10">
+      <c r="J59" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="10:10">
+      <c r="J60" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="10:10">
+      <c r="J61" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="10:10">
+      <c r="J62" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="10:10">
+      <c r="J63" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="10:10">
+      <c r="J64" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="10:10">
+      <c r="J65" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="10:10">
+      <c r="J66" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="10:10">
+      <c r="J67" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="10:10">
+      <c r="J68" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="10:10">
+      <c r="J69" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="10:10">
+      <c r="J70" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="10:10">
+      <c r="J71" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="10:10">
+      <c r="J72" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="10:10">
+      <c r="J73" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="10:10">
+      <c r="J74" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="10:10">
+      <c r="J75" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="10:10">
+      <c r="J76" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="10:10">
+      <c r="J77" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="10:10">
+      <c r="J78" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="10:10">
+      <c r="J79" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="10:10">
+      <c r="J80" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="10:10">
+      <c r="J81" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="10:10">
+      <c r="J82" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="10:10">
+      <c r="J83" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="10:10">
+      <c r="J84" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="10:10">
+      <c r="J85" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="10:10">
+      <c r="J86" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="10:10">
+      <c r="J87" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="10:10">
+      <c r="J88" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="10:10">
+      <c r="J89" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="10:10">
+      <c r="J90" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="10:10">
+      <c r="J91" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="10:10">
+      <c r="J92" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="10:10">
+      <c r="J93" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="10:10">
+      <c r="J94" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="10:10">
+      <c r="J95" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="10:10">
+      <c r="J96" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="10:10">
+      <c r="J97" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="10:10">
+      <c r="J98" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="10:10">
+      <c r="J99" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="10:10">
+      <c r="J100" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="10:10">
+      <c r="J101" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="10:10">
+      <c r="J102" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="10:10">
+      <c r="J103" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="10:10">
+      <c r="J104" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="10:10">
+      <c r="J105" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="10:10">
+      <c r="J106" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="10:10">
+      <c r="J107" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="10:10">
+      <c r="J108" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="10:10">
+      <c r="J109" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="10:10">
+      <c r="J110" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="10:10">
+      <c r="J111" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="10:10">
+      <c r="J112" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="10:10">
+      <c r="J113" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="10:10">
+      <c r="J114" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="10:10">
+      <c r="J115" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="10:10">
+      <c r="J116" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="10:10">
+      <c r="J117" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="10:10">
+      <c r="J118" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="10:10">
+      <c r="J119" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="10:10">
+      <c r="J120" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="10:10">
+      <c r="J121" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="10:10">
+      <c r="J122" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="123" spans="10:10">
+      <c r="J123" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="10:10">
+      <c r="J124" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="10:10">
+      <c r="J125" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="10:10">
+      <c r="J126" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="10:10">
+      <c r="J127" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="10:10">
+      <c r="J128" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="10:10">
+      <c r="J129" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="10:10">
+      <c r="J130" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="10:10">
+      <c r="J131" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="10:10">
+      <c r="J132" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="10:10">
+      <c r="J133" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="10:10">
+      <c r="J134" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="10:10">
+      <c r="J135" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="10:10">
+      <c r="J136" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="10:10">
+      <c r="J137" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="10:10">
+      <c r="J138" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="10:10">
+      <c r="J139" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="10:10">
+      <c r="J140" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="10:10">
+      <c r="J141" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="142" spans="10:10">
+      <c r="J142" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="10:10">
+      <c r="J143" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="10:10">
+      <c r="J144" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="10:10">
+      <c r="J145" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="10:10">
+      <c r="J146" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="10:10">
+      <c r="J147" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="10:10">
+      <c r="J148" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="10:10">
+      <c r="J149" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="10:10">
+      <c r="J150" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="10:10">
+      <c r="J151" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="10:10">
+      <c r="J152" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="10:10">
+      <c r="J153" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="10:10">
+      <c r="J154" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="10:10">
+      <c r="J155" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="10:10">
+      <c r="J156" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" spans="10:10">
+      <c r="J157" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="10:10">
+      <c r="J158" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="10:10">
+      <c r="J159" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="10:10">
+      <c r="J160" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161" spans="10:10">
+      <c r="J161" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="10:10">
+      <c r="J162" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="10:10">
+      <c r="J163" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="10:10">
+      <c r="J164" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="10:10">
+      <c r="J165" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="10:10">
+      <c r="J166" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="10:10">
+      <c r="J167" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="10:10">
+      <c r="J168" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="169" spans="10:10">
+      <c r="J169" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="10:10">
+      <c r="J170" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171" spans="10:10">
+      <c r="J171" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="10:10">
+      <c r="J172" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="10:10">
+      <c r="J173" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="174" spans="10:10">
+      <c r="J174" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="10:10">
+      <c r="J175" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="10:10">
+      <c r="J176" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="177" spans="10:10">
+      <c r="J177" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="10:10">
+      <c r="J178" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="179" spans="10:10">
+      <c r="J179" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="10:10">
+      <c r="J180" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="181" spans="10:10">
+      <c r="J181" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="182" spans="10:10">
+      <c r="J182" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="183" spans="10:10">
+      <c r="J183" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="10:10">
+      <c r="J184" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="185" spans="10:10">
+      <c r="J185" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="186" spans="10:10">
+      <c r="J186" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="187" spans="10:10">
+      <c r="J187" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="10:10">
+      <c r="J188" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189" spans="10:10">
+      <c r="J189" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190" spans="10:10">
+      <c r="J190" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191" spans="10:10">
+      <c r="J191" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="10:10">
+      <c r="J192" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193" spans="10:10">
+      <c r="J193" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="194" spans="10:10">
+      <c r="J194" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="10:10">
+      <c r="J195" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="10:10">
+      <c r="J196" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="197" spans="10:10">
+      <c r="J197" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="10:10">
+      <c r="J198" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="10:10">
+      <c r="J199" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="10:10">
+      <c r="J200" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="201" spans="10:10">
+      <c r="J201" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="10:10">
+      <c r="J202" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="203" spans="10:10">
+      <c r="J203" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="204" spans="10:10">
+      <c r="J204" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="10:10">
+      <c r="J205" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="206" spans="10:10">
+      <c r="J206" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="207" spans="10:10">
+      <c r="J207" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="208" spans="10:10">
+      <c r="J208" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="209" spans="10:10">
+      <c r="J209" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="10:10">
+      <c r="J210" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="211" spans="10:10">
+      <c r="J211" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="212" spans="10:10">
+      <c r="J212" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="213" spans="10:10">
+      <c r="J213" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="214" spans="10:10">
+      <c r="J214" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="215" spans="10:10">
+      <c r="J215" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="10:10">
+      <c r="J216" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="217" spans="10:10">
+      <c r="J217" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="218" spans="10:10">
+      <c r="J218" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="219" spans="10:10">
+      <c r="J219" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="10:10">
+      <c r="J220" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="221" spans="10:10">
+      <c r="J221" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="222" spans="10:10">
+      <c r="J222" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="223" spans="10:10">
+      <c r="J223" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="224" spans="10:10">
+      <c r="J224" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="225" spans="10:10">
+      <c r="J225" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="226" spans="10:10">
+      <c r="J226" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="227" spans="10:10">
+      <c r="J227" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="228" spans="10:10">
+      <c r="J228" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="229" spans="10:10">
+      <c r="J229" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="230" spans="10:10">
+      <c r="J230" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="231" spans="10:10">
+      <c r="J231" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="232" spans="10:10">
+      <c r="J232" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="233" spans="10:10">
+      <c r="J233" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="234" spans="10:10">
+      <c r="J234" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="235" spans="10:10">
+      <c r="J235" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="236" spans="10:10">
+      <c r="J236" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="237" spans="10:10">
+      <c r="J237" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="238" spans="10:10">
+      <c r="J238" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="10:10">
+      <c r="J239" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="240" spans="10:10">
+      <c r="J240" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="241" spans="10:10">
+      <c r="J241" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="242" spans="10:10">
+      <c r="J242" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="243" spans="10:10">
+      <c r="J243" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="10:10">
+      <c r="J244" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="10:10">
+      <c r="J245" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="246" spans="10:10">
+      <c r="J246" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="10:10">
+      <c r="J247" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="10:10">
+      <c r="J248" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="10:10">
+      <c r="J249" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="250" spans="10:10">
+      <c r="J250" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="10:10">
+      <c r="J251" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="10:10">
+      <c r="J252" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="253" spans="10:10">
+      <c r="J253" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254" spans="10:10">
+      <c r="J254" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="10:10">
+      <c r="J255" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256" spans="10:10">
+      <c r="J256" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="10:10">
+      <c r="J257" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="258" spans="10:10">
+      <c r="J258" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="259" spans="10:10">
+      <c r="J259" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="260" spans="10:10">
+      <c r="J260" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="261" spans="10:10">
+      <c r="J261" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="262" spans="10:10">
+      <c r="J262" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="263" spans="10:10">
+      <c r="J263" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="264" spans="10:10">
+      <c r="J264" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="265" spans="10:10">
+      <c r="J265" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="266" spans="10:10">
+      <c r="J266" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="267" spans="10:10">
+      <c r="J267" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="268" spans="10:10">
+      <c r="J268" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="269" spans="10:10">
+      <c r="J269" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="270" spans="10:10">
+      <c r="J270" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="271" spans="10:10">
+      <c r="J271" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="272" spans="10:10">
+      <c r="J272" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="273" spans="10:10">
+      <c r="J273" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="274" spans="10:10">
+      <c r="J274" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="275" spans="10:10">
+      <c r="J275" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="276" spans="10:10">
+      <c r="J276" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="277" spans="10:10">
+      <c r="J277" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="278" spans="10:10">
+      <c r="J278" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279" spans="10:10">
+      <c r="J279" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="280" spans="10:10">
+      <c r="J280" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281" spans="10:10">
+      <c r="J281" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="282" spans="10:10">
+      <c r="J282" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="283" spans="10:10">
+      <c r="J283" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="284" spans="10:10">
+      <c r="J284" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="285" spans="10:10">
+      <c r="J285" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="286" spans="10:10">
+      <c r="J286" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="287" spans="10:10">
+      <c r="J287" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="288" spans="10:10">
+      <c r="J288" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="289" spans="10:10">
+      <c r="J289" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="290" spans="10:10">
+      <c r="J290" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="291" spans="10:10">
+      <c r="J291" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="292" spans="10:10">
+      <c r="J292" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="293" spans="10:10">
+      <c r="J293" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="294" spans="10:10">
+      <c r="J294" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="295" spans="10:10">
+      <c r="J295" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="296" spans="10:10">
+      <c r="J296" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297" spans="10:10">
+      <c r="J297" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="298" spans="10:10">
+      <c r="J298" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="299" spans="10:10">
+      <c r="J299" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="300" spans="10:10">
+      <c r="J300" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="301" spans="10:10">
+      <c r="J301" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="302" spans="10:10">
+      <c r="J302" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="303" spans="10:10">
+      <c r="J303" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="304" spans="10:10">
+      <c r="J304" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="305" spans="10:10">
+      <c r="J305" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="306" spans="10:10">
+      <c r="J306" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="307" spans="10:10">
+      <c r="J307" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="308" spans="10:10">
+      <c r="J308" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="309" spans="10:10">
+      <c r="J309" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="310" spans="10:10">
+      <c r="J310" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="311" spans="10:10">
+      <c r="J311" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="312" spans="10:10">
+      <c r="J312" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="313" spans="10:10">
+      <c r="J313" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="314" spans="10:10">
+      <c r="J314" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="315" spans="10:10">
+      <c r="J315" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="316" spans="10:10">
+      <c r="J316" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="317" spans="10:10">
+      <c r="J317" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="318" spans="10:10">
+      <c r="J318" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="319" spans="10:10">
+      <c r="J319" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="320" spans="10:10">
+      <c r="J320" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="321" spans="10:10">
+      <c r="J321" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="322" spans="10:10">
+      <c r="J322" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="323" spans="10:10">
+      <c r="J323" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="324" spans="10:10">
+      <c r="J324" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="325" spans="10:10">
+      <c r="J325" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="326" spans="10:10">
+      <c r="J326" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="327" spans="10:10">
+      <c r="J327" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="328" spans="10:10">
+      <c r="J328" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="329" spans="10:10">
+      <c r="J329" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="330" spans="10:10">
+      <c r="J330" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="331" spans="10:10">
+      <c r="J331" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="332" spans="10:10">
+      <c r="J332" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="333" spans="10:10">
+      <c r="J333" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="334" spans="10:10">
+      <c r="J334" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="335" spans="10:10">
+      <c r="J335" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="336" spans="10:10">
+      <c r="J336" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="337" spans="10:10">
+      <c r="J337" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="338" spans="10:10">
+      <c r="J338" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="339" spans="10:10">
+      <c r="J339" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="340" spans="10:10">
+      <c r="J340" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="341" spans="10:10">
+      <c r="J341" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="342" spans="10:10">
+      <c r="J342" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="343" spans="10:10">
+      <c r="J343" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="344" spans="10:10">
+      <c r="J344" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="345" spans="10:10">
+      <c r="J345" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="346" spans="10:10">
+      <c r="J346" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="347" spans="10:10">
+      <c r="J347" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="348" spans="10:10">
+      <c r="J348" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="349" spans="10:10">
+      <c r="J349" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="350" spans="10:10">
+      <c r="J350" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="351" spans="10:10">
+      <c r="J351" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="352" spans="10:10">
+      <c r="J352" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="353" spans="10:10">
+      <c r="J353" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="354" spans="10:10">
+      <c r="J354" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="355" spans="10:10">
+      <c r="J355" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="356" spans="10:10">
+      <c r="J356" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="357" spans="10:10">
+      <c r="J357" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="358" spans="10:10">
+      <c r="J358" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="359" spans="10:10">
+      <c r="J359" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="360" spans="10:10">
+      <c r="J360" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="361" spans="10:10">
+      <c r="J361" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="362" spans="10:10">
+      <c r="J362" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="363" spans="10:10">
+      <c r="J363" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="364" spans="10:10">
+      <c r="J364" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="365" spans="10:10">
+      <c r="J365" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="366" spans="10:10">
+      <c r="J366" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="367" spans="10:10">
+      <c r="J367" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="368" spans="10:10">
+      <c r="J368" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="369" spans="10:10">
+      <c r="J369" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="370" spans="10:10">
+      <c r="J370" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="371" spans="10:10">
+      <c r="J371" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="372" spans="10:10">
+      <c r="J372" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="373" spans="10:10">
+      <c r="J373" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="374" spans="10:10">
+      <c r="J374" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="375" spans="10:10">
+      <c r="J375" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="376" spans="10:10">
+      <c r="J376" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="377" spans="10:10">
+      <c r="J377" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="378" spans="10:10">
+      <c r="J378" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="379" spans="10:10">
+      <c r="J379" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="380" spans="10:10">
+      <c r="J380" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="381" spans="10:10">
+      <c r="J381" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="382" spans="10:10">
+      <c r="J382" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="383" spans="10:10">
+      <c r="J383" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="384" spans="10:10">
+      <c r="J384" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="385" spans="10:10">
+      <c r="J385" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="386" spans="10:10">
+      <c r="J386" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="387" spans="10:10">
+      <c r="J387" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="388" spans="10:10">
+      <c r="J388" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="389" spans="10:10">
+      <c r="J389" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="390" spans="10:10">
+      <c r="J390" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="391" spans="10:10">
+      <c r="J391" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="392" spans="10:10">
+      <c r="J392" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="393" spans="10:10">
+      <c r="J393" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="394" spans="10:10">
+      <c r="J394" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="395" spans="10:10">
+      <c r="J395" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>